<commit_message>
2022/12/07 DB erd 설계 - 구홍모
</commit_message>
<xml_diff>
--- a/Kmarket API 설계.xlsx
+++ b/Kmarket API 설계.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\java1\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\java1\Desktop\Workspace\Kmarket1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -101,31 +101,31 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>http://localhost:8080/Kmarket/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://localhost:8080/Kmarket/index.do</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://localhost:8080/Kmarket/member/…</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://localhost:8080/Kmarket/product/…</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://localhost:8080/Kmarket/cs/…</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://localhost:8080/Kmarket/admin/…</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>홍길동</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>http://localhost:8080/Kmarket/</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>http://localhost:8080/Kmarket/index.do</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>http://localhost:8080/Kmarket/member/…</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>http://localhost:8080/Kmarket/product/…</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>http://localhost:8080/Kmarket/cs/…</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>http://localhost:8080/Kmarket/admin/…</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -519,7 +519,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -553,7 +553,7 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>3</v>
@@ -562,13 +562,13 @@
         <v>5</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="3"/>
       <c r="B3" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>3</v>
@@ -577,7 +577,7 @@
         <v>5</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -585,7 +585,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>3</v>
@@ -594,7 +594,7 @@
         <v>11</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -602,7 +602,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>3</v>
@@ -611,7 +611,7 @@
         <v>12</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -619,7 +619,7 @@
         <v>10</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>3</v>
@@ -628,7 +628,7 @@
         <v>13</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -636,7 +636,7 @@
         <v>9</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>3</v>
@@ -645,7 +645,7 @@
         <v>14</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>